<commit_message>
adding Pharo first slides
</commit_message>
<xml_diff>
--- a/HourLog.xlsx
+++ b/HourLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>before</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>started to hate slides :)</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>stef welcome</t>
+  </si>
+  <si>
+    <t>discussion with damien on the phone</t>
   </si>
 </sst>
 </file>
@@ -46,7 +58,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -70,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -416,24 +428,35 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="C1">
-        <f>SUM(B6:B19)</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>27</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
+        <f>SUM(B6:B29)</f>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>42192</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>42192</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
-        <v>26</v>
+      <c r="A7" s="1">
+        <v>42185</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -441,7 +464,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -449,65 +472,100 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>24</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
         <v>21</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B14">
+      <c r="B18">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B15">
+      <c r="B19">
         <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
         <v>250</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first pass on self sends next: 	factory 	hook and templates
</commit_message>
<xml_diff>
--- a/HourLog.xlsx
+++ b/HourLog.xlsx
@@ -418,7 +418,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -432,6 +432,14 @@
         <v>328</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>42207</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>42205</v>

</xml_diff>